<commit_message>
first commit since a wild (dev in local env)
</commit_message>
<xml_diff>
--- a/correlation_interpolation_get.xlsx
+++ b/correlation_interpolation_get.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,10 +466,15 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
+          <t>returns Private Equity USD Unhedged</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
           <t>returns UK Property Direct - USD Unhedged</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>returns unsmoothed</t>
         </is>
@@ -500,9 +505,12 @@
         <v>0.5598236069811342</v>
       </c>
       <c r="H2" t="n">
+        <v>0.5444423922450708</v>
+      </c>
+      <c r="I2" t="n">
         <v>0.4789715589445749</v>
       </c>
-      <c r="I2" t="n">
+      <c r="J2" t="n">
         <v>0.4947678149174207</v>
       </c>
     </row>
@@ -531,9 +539,12 @@
         <v>0.3349171384280981</v>
       </c>
       <c r="H3" t="n">
+        <v>0.9151257149970743</v>
+      </c>
+      <c r="I3" t="n">
         <v>0.8516054337564454</v>
       </c>
-      <c r="I3" t="n">
+      <c r="J3" t="n">
         <v>0.8241795568154309</v>
       </c>
     </row>
@@ -562,9 +573,12 @@
         <v>0.4462089699436975</v>
       </c>
       <c r="H4" t="n">
+        <v>0.8127456037382913</v>
+      </c>
+      <c r="I4" t="n">
         <v>0.6521731305310333</v>
       </c>
-      <c r="I4" t="n">
+      <c r="J4" t="n">
         <v>0.7600152792347502</v>
       </c>
     </row>
@@ -593,9 +607,12 @@
         <v>-0.2757287640025066</v>
       </c>
       <c r="H5" t="n">
+        <v>-0.1280087661092652</v>
+      </c>
+      <c r="I5" t="n">
         <v>-0.02013536346799655</v>
       </c>
-      <c r="I5" t="n">
+      <c r="J5" t="n">
         <v>-0.1209802626638477</v>
       </c>
     </row>
@@ -624,9 +641,12 @@
         <v>0.2370970856896036</v>
       </c>
       <c r="H6" t="n">
+        <v>0.7325619217938056</v>
+      </c>
+      <c r="I6" t="n">
         <v>0.7476820671256807</v>
       </c>
-      <c r="I6" t="n">
+      <c r="J6" t="n">
         <v>0.6589029409597525</v>
       </c>
     </row>
@@ -655,71 +675,114 @@
         <v>1</v>
       </c>
       <c r="H7" t="n">
+        <v>0.354584949574704</v>
+      </c>
+      <c r="I7" t="n">
         <v>0.3085737734152514</v>
       </c>
-      <c r="I7" t="n">
+      <c r="J7" t="n">
         <v>0.3393814822166029</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>returns UK Property Direct - USD Unhedged</t>
+          <t>returns Private Equity USD Unhedged</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.4789715589445749</v>
+        <v>0.5444423922450708</v>
       </c>
       <c r="C8" t="n">
-        <v>0.8516054337564454</v>
+        <v>0.9151257149970743</v>
       </c>
       <c r="D8" t="n">
-        <v>0.6521731305310333</v>
+        <v>0.8127456037382913</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.02013536346799655</v>
+        <v>-0.1280087661092652</v>
       </c>
       <c r="F8" t="n">
-        <v>0.7476820671256807</v>
+        <v>0.7325619217938056</v>
       </c>
       <c r="G8" t="n">
-        <v>0.3085737734152514</v>
+        <v>0.354584949574704</v>
       </c>
       <c r="H8" t="n">
         <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>0.7462332045979683</v>
+        <v>0.8552535606935843</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.875528909419702</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
+          <t>returns UK Property Direct - USD Unhedged</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.4789715589445749</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.8516054337564454</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.6521731305310333</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-0.02013536346799655</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.7476820671256807</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.3085737734152514</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.8552535606935843</v>
+      </c>
+      <c r="I9" t="n">
+        <v>1</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.7462332045979683</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
           <t>returns unsmoothed</t>
         </is>
       </c>
-      <c r="B9" t="n">
+      <c r="B10" t="n">
         <v>0.4947678149174207</v>
       </c>
-      <c r="C9" t="n">
+      <c r="C10" t="n">
         <v>0.8241795568154309</v>
       </c>
-      <c r="D9" t="n">
+      <c r="D10" t="n">
         <v>0.7600152792347502</v>
       </c>
-      <c r="E9" t="n">
+      <c r="E10" t="n">
         <v>-0.1209802626638477</v>
       </c>
-      <c r="F9" t="n">
+      <c r="F10" t="n">
         <v>0.6589029409597525</v>
       </c>
-      <c r="G9" t="n">
+      <c r="G10" t="n">
         <v>0.3393814822166029</v>
       </c>
-      <c r="H9" t="n">
+      <c r="H10" t="n">
+        <v>0.875528909419702</v>
+      </c>
+      <c r="I10" t="n">
         <v>0.7462332045979683</v>
       </c>
-      <c r="I9" t="n">
+      <c r="J10" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>